<commit_message>
he corregido un problema con la nomenclatura del embalse
</commit_message>
<xml_diff>
--- a/Excel/MUCVA+SIOSE_areas_usos.xlsx
+++ b/Excel/MUCVA+SIOSE_areas_usos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\TFM\rTFM\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\MASTER\TFM\rTFM\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8126" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8126" uniqueCount="345">
   <si>
     <t>fid</t>
   </si>
@@ -1030,9 +1030,6 @@
     <t>SIOSE2020</t>
   </si>
   <si>
-    <t>Cola del Embalse del NegratIn</t>
-  </si>
-  <si>
     <t>DIFERENCIA</t>
   </si>
   <si>
@@ -1690,47 +1687,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -10885,8 +10842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A840" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I794" sqref="I794:J865"/>
+    <sheetView tabSelected="1" topLeftCell="A363" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G386" sqref="G386:G409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10912,7 +10869,7 @@
         <v>151</v>
       </c>
       <c r="E1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F1" t="s">
         <v>327</v>
@@ -10924,10 +10881,10 @@
         <v>330</v>
       </c>
       <c r="I1" t="s">
+        <v>342</v>
+      </c>
+      <c r="J1" t="s">
         <v>343</v>
-      </c>
-      <c r="J1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -20091,7 +20048,7 @@
         <v>5</v>
       </c>
       <c r="F290" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G290" t="s">
         <v>144</v>
@@ -23166,7 +23123,7 @@
         <v>331</v>
       </c>
       <c r="G386" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H386">
         <v>0</v>
@@ -23198,7 +23155,7 @@
         <v>331</v>
       </c>
       <c r="G387" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H387">
         <v>1.052962</v>
@@ -23230,7 +23187,7 @@
         <v>331</v>
       </c>
       <c r="G388" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H388">
         <v>0</v>
@@ -23262,7 +23219,7 @@
         <v>331</v>
       </c>
       <c r="G389" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H389">
         <v>10.198543000000001</v>
@@ -23294,7 +23251,7 @@
         <v>331</v>
       </c>
       <c r="G390" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H390">
         <v>2.4969429999999999</v>
@@ -23326,7 +23283,7 @@
         <v>331</v>
       </c>
       <c r="G391" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H391">
         <v>0</v>
@@ -23358,7 +23315,7 @@
         <v>331</v>
       </c>
       <c r="G392" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H392">
         <v>0</v>
@@ -23390,7 +23347,7 @@
         <v>331</v>
       </c>
       <c r="G393" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H393">
         <v>0</v>
@@ -23422,7 +23379,7 @@
         <v>331</v>
       </c>
       <c r="G394" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H394">
         <v>0</v>
@@ -23454,7 +23411,7 @@
         <v>331</v>
       </c>
       <c r="G395" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H395">
         <v>0</v>
@@ -23486,7 +23443,7 @@
         <v>331</v>
       </c>
       <c r="G396" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H396">
         <v>0</v>
@@ -23518,7 +23475,7 @@
         <v>331</v>
       </c>
       <c r="G397" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H397">
         <v>90.983635000000007</v>
@@ -23550,7 +23507,7 @@
         <v>331</v>
       </c>
       <c r="G398" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H398">
         <v>0</v>
@@ -23582,7 +23539,7 @@
         <v>331</v>
       </c>
       <c r="G399" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H399">
         <v>179.84545499999999</v>
@@ -23614,7 +23571,7 @@
         <v>331</v>
       </c>
       <c r="G400" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H400">
         <v>139.291359</v>
@@ -23646,7 +23603,7 @@
         <v>331</v>
       </c>
       <c r="G401" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H401">
         <v>17.259428</v>
@@ -23678,7 +23635,7 @@
         <v>331</v>
       </c>
       <c r="G402" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H402">
         <v>0</v>
@@ -23710,7 +23667,7 @@
         <v>331</v>
       </c>
       <c r="G403" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H403">
         <v>82.479111000000003</v>
@@ -23742,7 +23699,7 @@
         <v>331</v>
       </c>
       <c r="G404" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H404">
         <v>0</v>
@@ -23774,7 +23731,7 @@
         <v>331</v>
       </c>
       <c r="G405" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H405">
         <v>266.46162800000002</v>
@@ -23806,7 +23763,7 @@
         <v>331</v>
       </c>
       <c r="G406" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H406">
         <v>0</v>
@@ -23838,7 +23795,7 @@
         <v>331</v>
       </c>
       <c r="G407" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H407">
         <v>0</v>
@@ -23870,7 +23827,7 @@
         <v>331</v>
       </c>
       <c r="G408" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H408">
         <v>60.986457999999999</v>
@@ -23902,7 +23859,7 @@
         <v>331</v>
       </c>
       <c r="G409" t="s">
-        <v>332</v>
+        <v>145</v>
       </c>
       <c r="H409">
         <v>0</v>
@@ -29307,7 +29264,7 @@
         <v>5</v>
       </c>
       <c r="F578" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G578" t="s">
         <v>144</v>
@@ -29339,7 +29296,7 @@
         <v>5</v>
       </c>
       <c r="F579" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G579" t="s">
         <v>144</v>
@@ -29371,7 +29328,7 @@
         <v>5</v>
       </c>
       <c r="F580" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G580" t="s">
         <v>144</v>
@@ -29403,7 +29360,7 @@
         <v>5</v>
       </c>
       <c r="F581" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G581" t="s">
         <v>144</v>
@@ -29435,7 +29392,7 @@
         <v>5</v>
       </c>
       <c r="F582" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G582" t="s">
         <v>144</v>
@@ -29467,7 +29424,7 @@
         <v>5</v>
       </c>
       <c r="F583" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G583" t="s">
         <v>144</v>
@@ -29499,7 +29456,7 @@
         <v>3</v>
       </c>
       <c r="F584" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G584" t="s">
         <v>144</v>
@@ -29531,7 +29488,7 @@
         <v>1</v>
       </c>
       <c r="F585" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G585" t="s">
         <v>144</v>
@@ -29563,7 +29520,7 @@
         <v>1</v>
       </c>
       <c r="F586" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G586" t="s">
         <v>144</v>
@@ -29595,7 +29552,7 @@
         <v>1</v>
       </c>
       <c r="F587" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G587" t="s">
         <v>144</v>
@@ -29627,7 +29584,7 @@
         <v>1</v>
       </c>
       <c r="F588" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G588" t="s">
         <v>144</v>
@@ -29659,7 +29616,7 @@
         <v>1</v>
       </c>
       <c r="F589" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G589" t="s">
         <v>144</v>
@@ -29691,7 +29648,7 @@
         <v>1</v>
       </c>
       <c r="F590" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G590" t="s">
         <v>144</v>
@@ -29723,7 +29680,7 @@
         <v>4</v>
       </c>
       <c r="F591" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G591" t="s">
         <v>144</v>
@@ -29755,7 +29712,7 @@
         <v>3</v>
       </c>
       <c r="F592" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G592" t="s">
         <v>144</v>
@@ -29787,7 +29744,7 @@
         <v>3</v>
       </c>
       <c r="F593" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G593" t="s">
         <v>144</v>
@@ -29819,7 +29776,7 @@
         <v>5</v>
       </c>
       <c r="F594" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G594" t="s">
         <v>144</v>
@@ -29851,7 +29808,7 @@
         <v>3</v>
       </c>
       <c r="F595" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G595" t="s">
         <v>144</v>
@@ -29883,7 +29840,7 @@
         <v>3</v>
       </c>
       <c r="F596" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G596" t="s">
         <v>144</v>
@@ -29915,7 +29872,7 @@
         <v>1</v>
       </c>
       <c r="F597" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G597" t="s">
         <v>144</v>
@@ -29947,7 +29904,7 @@
         <v>2</v>
       </c>
       <c r="F598" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G598" t="s">
         <v>144</v>
@@ -29979,7 +29936,7 @@
         <v>1</v>
       </c>
       <c r="F599" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G599" t="s">
         <v>144</v>
@@ -30011,7 +29968,7 @@
         <v>1</v>
       </c>
       <c r="F600" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G600" t="s">
         <v>144</v>
@@ -30043,7 +30000,7 @@
         <v>4</v>
       </c>
       <c r="F601" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G601" t="s">
         <v>144</v>
@@ -30075,7 +30032,7 @@
         <v>5</v>
       </c>
       <c r="F602" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G602" t="s">
         <v>117</v>
@@ -30107,7 +30064,7 @@
         <v>5</v>
       </c>
       <c r="F603" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G603" t="s">
         <v>117</v>
@@ -30139,7 +30096,7 @@
         <v>5</v>
       </c>
       <c r="F604" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G604" t="s">
         <v>117</v>
@@ -30171,7 +30128,7 @@
         <v>5</v>
       </c>
       <c r="F605" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G605" t="s">
         <v>117</v>
@@ -30203,7 +30160,7 @@
         <v>5</v>
       </c>
       <c r="F606" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G606" t="s">
         <v>117</v>
@@ -30235,7 +30192,7 @@
         <v>5</v>
       </c>
       <c r="F607" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G607" t="s">
         <v>117</v>
@@ -30267,7 +30224,7 @@
         <v>3</v>
       </c>
       <c r="F608" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G608" t="s">
         <v>117</v>
@@ -30299,7 +30256,7 @@
         <v>1</v>
       </c>
       <c r="F609" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G609" t="s">
         <v>117</v>
@@ -30331,7 +30288,7 @@
         <v>1</v>
       </c>
       <c r="F610" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G610" t="s">
         <v>117</v>
@@ -30363,7 +30320,7 @@
         <v>1</v>
       </c>
       <c r="F611" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G611" t="s">
         <v>117</v>
@@ -30395,7 +30352,7 @@
         <v>1</v>
       </c>
       <c r="F612" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G612" t="s">
         <v>117</v>
@@ -30427,7 +30384,7 @@
         <v>1</v>
       </c>
       <c r="F613" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G613" t="s">
         <v>117</v>
@@ -30459,7 +30416,7 @@
         <v>1</v>
       </c>
       <c r="F614" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G614" t="s">
         <v>117</v>
@@ -30491,7 +30448,7 @@
         <v>4</v>
       </c>
       <c r="F615" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G615" t="s">
         <v>117</v>
@@ -30523,7 +30480,7 @@
         <v>3</v>
       </c>
       <c r="F616" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G616" t="s">
         <v>117</v>
@@ -30555,7 +30512,7 @@
         <v>3</v>
       </c>
       <c r="F617" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G617" t="s">
         <v>117</v>
@@ -30587,7 +30544,7 @@
         <v>5</v>
       </c>
       <c r="F618" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G618" t="s">
         <v>117</v>
@@ -30619,7 +30576,7 @@
         <v>3</v>
       </c>
       <c r="F619" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G619" t="s">
         <v>117</v>
@@ -30651,7 +30608,7 @@
         <v>3</v>
       </c>
       <c r="F620" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G620" t="s">
         <v>117</v>
@@ -30683,7 +30640,7 @@
         <v>1</v>
       </c>
       <c r="F621" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G621" t="s">
         <v>117</v>
@@ -30715,7 +30672,7 @@
         <v>2</v>
       </c>
       <c r="F622" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G622" t="s">
         <v>117</v>
@@ -30747,7 +30704,7 @@
         <v>1</v>
       </c>
       <c r="F623" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G623" t="s">
         <v>117</v>
@@ -30779,7 +30736,7 @@
         <v>1</v>
       </c>
       <c r="F624" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G624" t="s">
         <v>117</v>
@@ -30811,7 +30768,7 @@
         <v>4</v>
       </c>
       <c r="F625" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G625" t="s">
         <v>117</v>
@@ -30843,7 +30800,7 @@
         <v>5</v>
       </c>
       <c r="F626" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G626" t="s">
         <v>165</v>
@@ -30875,7 +30832,7 @@
         <v>5</v>
       </c>
       <c r="F627" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G627" t="s">
         <v>165</v>
@@ -30907,7 +30864,7 @@
         <v>5</v>
       </c>
       <c r="F628" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G628" t="s">
         <v>165</v>
@@ -30939,7 +30896,7 @@
         <v>5</v>
       </c>
       <c r="F629" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G629" t="s">
         <v>165</v>
@@ -30971,7 +30928,7 @@
         <v>5</v>
       </c>
       <c r="F630" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G630" t="s">
         <v>165</v>
@@ -31003,7 +30960,7 @@
         <v>5</v>
       </c>
       <c r="F631" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G631" t="s">
         <v>165</v>
@@ -31035,7 +30992,7 @@
         <v>3</v>
       </c>
       <c r="F632" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G632" t="s">
         <v>165</v>
@@ -31067,7 +31024,7 @@
         <v>1</v>
       </c>
       <c r="F633" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G633" t="s">
         <v>165</v>
@@ -31099,7 +31056,7 @@
         <v>1</v>
       </c>
       <c r="F634" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G634" t="s">
         <v>165</v>
@@ -31131,7 +31088,7 @@
         <v>1</v>
       </c>
       <c r="F635" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G635" t="s">
         <v>165</v>
@@ -31163,7 +31120,7 @@
         <v>1</v>
       </c>
       <c r="F636" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G636" t="s">
         <v>165</v>
@@ -31195,7 +31152,7 @@
         <v>1</v>
       </c>
       <c r="F637" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G637" t="s">
         <v>165</v>
@@ -31227,7 +31184,7 @@
         <v>1</v>
       </c>
       <c r="F638" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G638" t="s">
         <v>165</v>
@@ -31259,7 +31216,7 @@
         <v>4</v>
       </c>
       <c r="F639" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G639" t="s">
         <v>165</v>
@@ -31291,7 +31248,7 @@
         <v>3</v>
       </c>
       <c r="F640" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G640" t="s">
         <v>165</v>
@@ -31323,7 +31280,7 @@
         <v>3</v>
       </c>
       <c r="F641" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G641" t="s">
         <v>165</v>
@@ -31355,7 +31312,7 @@
         <v>5</v>
       </c>
       <c r="F642" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G642" t="s">
         <v>165</v>
@@ -31387,7 +31344,7 @@
         <v>3</v>
       </c>
       <c r="F643" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G643" t="s">
         <v>165</v>
@@ -31419,7 +31376,7 @@
         <v>3</v>
       </c>
       <c r="F644" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G644" t="s">
         <v>165</v>
@@ -31451,7 +31408,7 @@
         <v>1</v>
       </c>
       <c r="F645" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G645" t="s">
         <v>165</v>
@@ -31483,7 +31440,7 @@
         <v>2</v>
       </c>
       <c r="F646" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G646" t="s">
         <v>165</v>
@@ -31515,7 +31472,7 @@
         <v>1</v>
       </c>
       <c r="F647" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G647" t="s">
         <v>165</v>
@@ -31547,7 +31504,7 @@
         <v>1</v>
       </c>
       <c r="F648" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G648" t="s">
         <v>165</v>
@@ -31579,7 +31536,7 @@
         <v>4</v>
       </c>
       <c r="F649" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G649" t="s">
         <v>165</v>
@@ -31611,7 +31568,7 @@
         <v>5</v>
       </c>
       <c r="F650" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G650" t="s">
         <v>45</v>
@@ -31643,7 +31600,7 @@
         <v>5</v>
       </c>
       <c r="F651" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G651" t="s">
         <v>45</v>
@@ -31675,7 +31632,7 @@
         <v>5</v>
       </c>
       <c r="F652" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G652" t="s">
         <v>45</v>
@@ -31707,7 +31664,7 @@
         <v>5</v>
       </c>
       <c r="F653" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G653" t="s">
         <v>45</v>
@@ -31739,7 +31696,7 @@
         <v>5</v>
       </c>
       <c r="F654" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G654" t="s">
         <v>45</v>
@@ -31771,7 +31728,7 @@
         <v>5</v>
       </c>
       <c r="F655" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G655" t="s">
         <v>45</v>
@@ -31803,7 +31760,7 @@
         <v>3</v>
       </c>
       <c r="F656" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G656" t="s">
         <v>45</v>
@@ -31835,7 +31792,7 @@
         <v>1</v>
       </c>
       <c r="F657" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G657" t="s">
         <v>45</v>
@@ -31867,7 +31824,7 @@
         <v>1</v>
       </c>
       <c r="F658" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G658" t="s">
         <v>45</v>
@@ -31899,7 +31856,7 @@
         <v>1</v>
       </c>
       <c r="F659" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G659" t="s">
         <v>45</v>
@@ -31931,7 +31888,7 @@
         <v>1</v>
       </c>
       <c r="F660" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G660" t="s">
         <v>45</v>
@@ -31963,7 +31920,7 @@
         <v>1</v>
       </c>
       <c r="F661" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G661" t="s">
         <v>45</v>
@@ -31995,7 +31952,7 @@
         <v>1</v>
       </c>
       <c r="F662" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G662" t="s">
         <v>45</v>
@@ -32027,7 +31984,7 @@
         <v>4</v>
       </c>
       <c r="F663" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G663" t="s">
         <v>45</v>
@@ -32059,7 +32016,7 @@
         <v>3</v>
       </c>
       <c r="F664" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G664" t="s">
         <v>45</v>
@@ -32091,7 +32048,7 @@
         <v>3</v>
       </c>
       <c r="F665" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G665" t="s">
         <v>45</v>
@@ -32123,7 +32080,7 @@
         <v>5</v>
       </c>
       <c r="F666" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G666" t="s">
         <v>45</v>
@@ -32155,7 +32112,7 @@
         <v>3</v>
       </c>
       <c r="F667" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G667" t="s">
         <v>45</v>
@@ -32187,7 +32144,7 @@
         <v>3</v>
       </c>
       <c r="F668" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G668" t="s">
         <v>45</v>
@@ -32219,7 +32176,7 @@
         <v>1</v>
       </c>
       <c r="F669" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G669" t="s">
         <v>45</v>
@@ -32251,7 +32208,7 @@
         <v>2</v>
       </c>
       <c r="F670" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G670" t="s">
         <v>45</v>
@@ -32283,7 +32240,7 @@
         <v>1</v>
       </c>
       <c r="F671" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G671" t="s">
         <v>45</v>
@@ -32315,7 +32272,7 @@
         <v>1</v>
       </c>
       <c r="F672" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G672" t="s">
         <v>45</v>
@@ -32347,7 +32304,7 @@
         <v>4</v>
       </c>
       <c r="F673" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G673" t="s">
         <v>45</v>
@@ -32379,7 +32336,7 @@
         <v>5</v>
       </c>
       <c r="F674" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G674" t="s">
         <v>145</v>
@@ -32411,7 +32368,7 @@
         <v>5</v>
       </c>
       <c r="F675" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G675" t="s">
         <v>145</v>
@@ -32443,7 +32400,7 @@
         <v>5</v>
       </c>
       <c r="F676" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G676" t="s">
         <v>145</v>
@@ -32475,7 +32432,7 @@
         <v>5</v>
       </c>
       <c r="F677" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G677" t="s">
         <v>145</v>
@@ -32507,7 +32464,7 @@
         <v>5</v>
       </c>
       <c r="F678" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G678" t="s">
         <v>145</v>
@@ -32539,7 +32496,7 @@
         <v>5</v>
       </c>
       <c r="F679" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G679" t="s">
         <v>145</v>
@@ -32571,7 +32528,7 @@
         <v>3</v>
       </c>
       <c r="F680" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G680" t="s">
         <v>145</v>
@@ -32603,7 +32560,7 @@
         <v>1</v>
       </c>
       <c r="F681" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G681" t="s">
         <v>145</v>
@@ -32635,7 +32592,7 @@
         <v>1</v>
       </c>
       <c r="F682" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G682" t="s">
         <v>145</v>
@@ -32667,7 +32624,7 @@
         <v>1</v>
       </c>
       <c r="F683" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G683" t="s">
         <v>145</v>
@@ -32699,7 +32656,7 @@
         <v>1</v>
       </c>
       <c r="F684" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G684" t="s">
         <v>145</v>
@@ -32731,7 +32688,7 @@
         <v>1</v>
       </c>
       <c r="F685" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G685" t="s">
         <v>145</v>
@@ -32763,7 +32720,7 @@
         <v>1</v>
       </c>
       <c r="F686" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G686" t="s">
         <v>145</v>
@@ -32795,7 +32752,7 @@
         <v>4</v>
       </c>
       <c r="F687" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G687" t="s">
         <v>145</v>
@@ -32827,7 +32784,7 @@
         <v>3</v>
       </c>
       <c r="F688" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G688" t="s">
         <v>145</v>
@@ -32859,7 +32816,7 @@
         <v>3</v>
       </c>
       <c r="F689" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G689" t="s">
         <v>145</v>
@@ -32891,7 +32848,7 @@
         <v>5</v>
       </c>
       <c r="F690" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G690" t="s">
         <v>145</v>
@@ -32923,7 +32880,7 @@
         <v>3</v>
       </c>
       <c r="F691" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G691" t="s">
         <v>145</v>
@@ -32955,7 +32912,7 @@
         <v>3</v>
       </c>
       <c r="F692" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G692" t="s">
         <v>145</v>
@@ -32987,7 +32944,7 @@
         <v>1</v>
       </c>
       <c r="F693" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G693" t="s">
         <v>145</v>
@@ -33019,7 +32976,7 @@
         <v>2</v>
       </c>
       <c r="F694" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G694" t="s">
         <v>145</v>
@@ -33051,7 +33008,7 @@
         <v>1</v>
       </c>
       <c r="F695" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G695" t="s">
         <v>145</v>
@@ -33083,7 +33040,7 @@
         <v>1</v>
       </c>
       <c r="F696" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G696" t="s">
         <v>145</v>
@@ -33115,7 +33072,7 @@
         <v>4</v>
       </c>
       <c r="F697" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G697" t="s">
         <v>145</v>
@@ -33147,7 +33104,7 @@
         <v>5</v>
       </c>
       <c r="F698" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G698" t="s">
         <v>78</v>
@@ -33179,7 +33136,7 @@
         <v>5</v>
       </c>
       <c r="F699" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G699" t="s">
         <v>78</v>
@@ -33211,7 +33168,7 @@
         <v>5</v>
       </c>
       <c r="F700" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G700" t="s">
         <v>78</v>
@@ -33243,7 +33200,7 @@
         <v>5</v>
       </c>
       <c r="F701" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G701" t="s">
         <v>78</v>
@@ -33275,7 +33232,7 @@
         <v>5</v>
       </c>
       <c r="F702" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G702" t="s">
         <v>78</v>
@@ -33307,7 +33264,7 @@
         <v>5</v>
       </c>
       <c r="F703" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G703" t="s">
         <v>78</v>
@@ -33339,7 +33296,7 @@
         <v>3</v>
       </c>
       <c r="F704" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G704" t="s">
         <v>78</v>
@@ -33371,7 +33328,7 @@
         <v>1</v>
       </c>
       <c r="F705" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G705" t="s">
         <v>78</v>
@@ -33403,7 +33360,7 @@
         <v>1</v>
       </c>
       <c r="F706" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G706" t="s">
         <v>78</v>
@@ -33435,7 +33392,7 @@
         <v>1</v>
       </c>
       <c r="F707" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G707" t="s">
         <v>78</v>
@@ -33467,7 +33424,7 @@
         <v>1</v>
       </c>
       <c r="F708" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G708" t="s">
         <v>78</v>
@@ -33499,7 +33456,7 @@
         <v>1</v>
       </c>
       <c r="F709" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G709" t="s">
         <v>78</v>
@@ -33531,7 +33488,7 @@
         <v>1</v>
       </c>
       <c r="F710" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G710" t="s">
         <v>78</v>
@@ -33563,7 +33520,7 @@
         <v>4</v>
       </c>
       <c r="F711" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G711" t="s">
         <v>78</v>
@@ -33595,7 +33552,7 @@
         <v>3</v>
       </c>
       <c r="F712" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G712" t="s">
         <v>78</v>
@@ -33627,7 +33584,7 @@
         <v>3</v>
       </c>
       <c r="F713" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G713" t="s">
         <v>78</v>
@@ -33659,7 +33616,7 @@
         <v>5</v>
       </c>
       <c r="F714" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G714" t="s">
         <v>78</v>
@@ -33691,7 +33648,7 @@
         <v>3</v>
       </c>
       <c r="F715" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G715" t="s">
         <v>78</v>
@@ -33723,7 +33680,7 @@
         <v>3</v>
       </c>
       <c r="F716" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G716" t="s">
         <v>78</v>
@@ -33755,7 +33712,7 @@
         <v>1</v>
       </c>
       <c r="F717" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G717" t="s">
         <v>78</v>
@@ -33787,7 +33744,7 @@
         <v>2</v>
       </c>
       <c r="F718" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G718" t="s">
         <v>78</v>
@@ -33819,7 +33776,7 @@
         <v>1</v>
       </c>
       <c r="F719" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G719" t="s">
         <v>78</v>
@@ -33851,7 +33808,7 @@
         <v>1</v>
       </c>
       <c r="F720" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G720" t="s">
         <v>78</v>
@@ -33883,7 +33840,7 @@
         <v>4</v>
       </c>
       <c r="F721" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G721" t="s">
         <v>78</v>
@@ -33915,7 +33872,7 @@
         <v>5</v>
       </c>
       <c r="F722" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G722" t="s">
         <v>100</v>
@@ -33947,7 +33904,7 @@
         <v>5</v>
       </c>
       <c r="F723" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G723" t="s">
         <v>100</v>
@@ -33979,7 +33936,7 @@
         <v>5</v>
       </c>
       <c r="F724" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G724" t="s">
         <v>100</v>
@@ -34011,7 +33968,7 @@
         <v>5</v>
       </c>
       <c r="F725" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G725" t="s">
         <v>100</v>
@@ -34043,7 +34000,7 @@
         <v>5</v>
       </c>
       <c r="F726" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G726" t="s">
         <v>100</v>
@@ -34075,7 +34032,7 @@
         <v>5</v>
       </c>
       <c r="F727" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G727" t="s">
         <v>100</v>
@@ -34107,7 +34064,7 @@
         <v>3</v>
       </c>
       <c r="F728" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G728" t="s">
         <v>100</v>
@@ -34139,7 +34096,7 @@
         <v>1</v>
       </c>
       <c r="F729" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G729" t="s">
         <v>100</v>
@@ -34171,7 +34128,7 @@
         <v>1</v>
       </c>
       <c r="F730" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G730" t="s">
         <v>100</v>
@@ -34203,7 +34160,7 @@
         <v>1</v>
       </c>
       <c r="F731" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G731" t="s">
         <v>100</v>
@@ -34235,7 +34192,7 @@
         <v>1</v>
       </c>
       <c r="F732" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G732" t="s">
         <v>100</v>
@@ -34267,7 +34224,7 @@
         <v>1</v>
       </c>
       <c r="F733" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G733" t="s">
         <v>100</v>
@@ -34299,7 +34256,7 @@
         <v>1</v>
       </c>
       <c r="F734" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G734" t="s">
         <v>100</v>
@@ -34331,7 +34288,7 @@
         <v>4</v>
       </c>
       <c r="F735" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G735" t="s">
         <v>100</v>
@@ -34363,7 +34320,7 @@
         <v>3</v>
       </c>
       <c r="F736" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G736" t="s">
         <v>100</v>
@@ -34395,7 +34352,7 @@
         <v>3</v>
       </c>
       <c r="F737" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G737" t="s">
         <v>100</v>
@@ -34427,7 +34384,7 @@
         <v>5</v>
       </c>
       <c r="F738" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G738" t="s">
         <v>100</v>
@@ -34459,7 +34416,7 @@
         <v>3</v>
       </c>
       <c r="F739" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G739" t="s">
         <v>100</v>
@@ -34491,7 +34448,7 @@
         <v>3</v>
       </c>
       <c r="F740" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G740" t="s">
         <v>100</v>
@@ -34523,7 +34480,7 @@
         <v>1</v>
       </c>
       <c r="F741" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G741" t="s">
         <v>100</v>
@@ -34555,7 +34512,7 @@
         <v>2</v>
       </c>
       <c r="F742" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G742" t="s">
         <v>100</v>
@@ -34587,7 +34544,7 @@
         <v>1</v>
       </c>
       <c r="F743" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G743" t="s">
         <v>100</v>
@@ -34619,7 +34576,7 @@
         <v>1</v>
       </c>
       <c r="F744" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G744" t="s">
         <v>100</v>
@@ -34651,7 +34608,7 @@
         <v>4</v>
       </c>
       <c r="F745" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G745" t="s">
         <v>100</v>
@@ -34683,7 +34640,7 @@
         <v>5</v>
       </c>
       <c r="F746" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G746" t="s">
         <v>87</v>
@@ -34715,7 +34672,7 @@
         <v>5</v>
       </c>
       <c r="F747" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G747" t="s">
         <v>87</v>
@@ -34747,7 +34704,7 @@
         <v>5</v>
       </c>
       <c r="F748" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G748" t="s">
         <v>87</v>
@@ -34779,7 +34736,7 @@
         <v>5</v>
       </c>
       <c r="F749" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G749" t="s">
         <v>87</v>
@@ -34811,7 +34768,7 @@
         <v>5</v>
       </c>
       <c r="F750" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G750" t="s">
         <v>87</v>
@@ -34843,7 +34800,7 @@
         <v>5</v>
       </c>
       <c r="F751" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G751" t="s">
         <v>87</v>
@@ -34875,7 +34832,7 @@
         <v>3</v>
       </c>
       <c r="F752" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G752" t="s">
         <v>87</v>
@@ -34907,7 +34864,7 @@
         <v>1</v>
       </c>
       <c r="F753" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G753" t="s">
         <v>87</v>
@@ -34939,7 +34896,7 @@
         <v>1</v>
       </c>
       <c r="F754" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G754" t="s">
         <v>87</v>
@@ -34971,7 +34928,7 @@
         <v>1</v>
       </c>
       <c r="F755" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G755" t="s">
         <v>87</v>
@@ -35003,7 +34960,7 @@
         <v>1</v>
       </c>
       <c r="F756" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G756" t="s">
         <v>87</v>
@@ -35035,7 +34992,7 @@
         <v>1</v>
       </c>
       <c r="F757" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G757" t="s">
         <v>87</v>
@@ -35067,7 +35024,7 @@
         <v>1</v>
       </c>
       <c r="F758" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G758" t="s">
         <v>87</v>
@@ -35099,7 +35056,7 @@
         <v>4</v>
       </c>
       <c r="F759" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G759" t="s">
         <v>87</v>
@@ -35131,7 +35088,7 @@
         <v>3</v>
       </c>
       <c r="F760" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G760" t="s">
         <v>87</v>
@@ -35163,7 +35120,7 @@
         <v>3</v>
       </c>
       <c r="F761" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G761" t="s">
         <v>87</v>
@@ -35195,7 +35152,7 @@
         <v>5</v>
       </c>
       <c r="F762" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G762" t="s">
         <v>87</v>
@@ -35227,7 +35184,7 @@
         <v>3</v>
       </c>
       <c r="F763" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G763" t="s">
         <v>87</v>
@@ -35259,7 +35216,7 @@
         <v>3</v>
       </c>
       <c r="F764" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G764" t="s">
         <v>87</v>
@@ -35291,7 +35248,7 @@
         <v>1</v>
       </c>
       <c r="F765" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G765" t="s">
         <v>87</v>
@@ -35323,7 +35280,7 @@
         <v>2</v>
       </c>
       <c r="F766" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G766" t="s">
         <v>87</v>
@@ -35355,7 +35312,7 @@
         <v>1</v>
       </c>
       <c r="F767" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G767" t="s">
         <v>87</v>
@@ -35387,7 +35344,7 @@
         <v>1</v>
       </c>
       <c r="F768" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G768" t="s">
         <v>87</v>
@@ -35419,7 +35376,7 @@
         <v>4</v>
       </c>
       <c r="F769" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G769" t="s">
         <v>87</v>
@@ -35451,7 +35408,7 @@
         <v>5</v>
       </c>
       <c r="F770" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G770" t="s">
         <v>147</v>
@@ -35483,7 +35440,7 @@
         <v>5</v>
       </c>
       <c r="F771" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G771" t="s">
         <v>147</v>
@@ -35515,7 +35472,7 @@
         <v>5</v>
       </c>
       <c r="F772" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G772" t="s">
         <v>147</v>
@@ -35547,7 +35504,7 @@
         <v>5</v>
       </c>
       <c r="F773" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G773" t="s">
         <v>147</v>
@@ -35579,7 +35536,7 @@
         <v>5</v>
       </c>
       <c r="F774" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G774" t="s">
         <v>147</v>
@@ -35611,7 +35568,7 @@
         <v>5</v>
       </c>
       <c r="F775" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G775" t="s">
         <v>147</v>
@@ -35643,7 +35600,7 @@
         <v>3</v>
       </c>
       <c r="F776" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G776" t="s">
         <v>147</v>
@@ -35675,7 +35632,7 @@
         <v>1</v>
       </c>
       <c r="F777" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G777" t="s">
         <v>147</v>
@@ -35707,7 +35664,7 @@
         <v>1</v>
       </c>
       <c r="F778" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G778" t="s">
         <v>147</v>
@@ -35739,7 +35696,7 @@
         <v>1</v>
       </c>
       <c r="F779" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G779" t="s">
         <v>147</v>
@@ -35771,7 +35728,7 @@
         <v>1</v>
       </c>
       <c r="F780" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G780" t="s">
         <v>147</v>
@@ -35803,7 +35760,7 @@
         <v>1</v>
       </c>
       <c r="F781" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G781" t="s">
         <v>147</v>
@@ -35835,7 +35792,7 @@
         <v>1</v>
       </c>
       <c r="F782" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G782" t="s">
         <v>147</v>
@@ -35867,7 +35824,7 @@
         <v>4</v>
       </c>
       <c r="F783" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G783" t="s">
         <v>147</v>
@@ -35899,7 +35856,7 @@
         <v>3</v>
       </c>
       <c r="F784" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G784" t="s">
         <v>147</v>
@@ -35931,7 +35888,7 @@
         <v>3</v>
       </c>
       <c r="F785" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G785" t="s">
         <v>147</v>
@@ -35963,7 +35920,7 @@
         <v>5</v>
       </c>
       <c r="F786" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G786" t="s">
         <v>147</v>
@@ -35995,7 +35952,7 @@
         <v>3</v>
       </c>
       <c r="F787" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G787" t="s">
         <v>147</v>
@@ -36027,7 +35984,7 @@
         <v>3</v>
       </c>
       <c r="F788" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G788" t="s">
         <v>147</v>
@@ -36059,7 +36016,7 @@
         <v>1</v>
       </c>
       <c r="F789" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G789" t="s">
         <v>147</v>
@@ -36091,7 +36048,7 @@
         <v>2</v>
       </c>
       <c r="F790" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G790" t="s">
         <v>147</v>
@@ -36123,7 +36080,7 @@
         <v>1</v>
       </c>
       <c r="F791" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G791" t="s">
         <v>147</v>
@@ -36155,7 +36112,7 @@
         <v>1</v>
       </c>
       <c r="F792" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G792" t="s">
         <v>147</v>
@@ -36187,7 +36144,7 @@
         <v>4</v>
       </c>
       <c r="F793" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G793" t="s">
         <v>147</v>
@@ -36219,7 +36176,7 @@
         <v>5</v>
       </c>
       <c r="F794" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G794" t="s">
         <v>27</v>
@@ -36251,7 +36208,7 @@
         <v>5</v>
       </c>
       <c r="F795" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G795" t="s">
         <v>27</v>
@@ -36283,7 +36240,7 @@
         <v>5</v>
       </c>
       <c r="F796" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G796" t="s">
         <v>27</v>
@@ -36315,7 +36272,7 @@
         <v>5</v>
       </c>
       <c r="F797" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G797" t="s">
         <v>27</v>
@@ -36347,7 +36304,7 @@
         <v>5</v>
       </c>
       <c r="F798" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G798" t="s">
         <v>27</v>
@@ -36379,7 +36336,7 @@
         <v>5</v>
       </c>
       <c r="F799" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G799" t="s">
         <v>27</v>
@@ -36411,7 +36368,7 @@
         <v>3</v>
       </c>
       <c r="F800" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G800" t="s">
         <v>27</v>
@@ -36443,7 +36400,7 @@
         <v>1</v>
       </c>
       <c r="F801" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G801" t="s">
         <v>27</v>
@@ -36475,7 +36432,7 @@
         <v>1</v>
       </c>
       <c r="F802" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G802" t="s">
         <v>27</v>
@@ -36507,7 +36464,7 @@
         <v>1</v>
       </c>
       <c r="F803" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G803" t="s">
         <v>27</v>
@@ -36539,7 +36496,7 @@
         <v>1</v>
       </c>
       <c r="F804" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G804" t="s">
         <v>27</v>
@@ -36571,7 +36528,7 @@
         <v>1</v>
       </c>
       <c r="F805" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G805" t="s">
         <v>27</v>
@@ -36603,7 +36560,7 @@
         <v>1</v>
       </c>
       <c r="F806" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G806" t="s">
         <v>27</v>
@@ -36635,7 +36592,7 @@
         <v>4</v>
       </c>
       <c r="F807" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G807" t="s">
         <v>27</v>
@@ -36667,7 +36624,7 @@
         <v>3</v>
       </c>
       <c r="F808" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G808" t="s">
         <v>27</v>
@@ -36699,7 +36656,7 @@
         <v>3</v>
       </c>
       <c r="F809" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G809" t="s">
         <v>27</v>
@@ -36731,7 +36688,7 @@
         <v>5</v>
       </c>
       <c r="F810" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G810" t="s">
         <v>27</v>
@@ -36763,7 +36720,7 @@
         <v>3</v>
       </c>
       <c r="F811" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G811" t="s">
         <v>27</v>
@@ -36795,7 +36752,7 @@
         <v>3</v>
       </c>
       <c r="F812" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G812" t="s">
         <v>27</v>
@@ -36827,7 +36784,7 @@
         <v>1</v>
       </c>
       <c r="F813" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G813" t="s">
         <v>27</v>
@@ -36859,7 +36816,7 @@
         <v>2</v>
       </c>
       <c r="F814" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G814" t="s">
         <v>27</v>
@@ -36891,7 +36848,7 @@
         <v>1</v>
       </c>
       <c r="F815" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G815" t="s">
         <v>27</v>
@@ -36923,7 +36880,7 @@
         <v>1</v>
       </c>
       <c r="F816" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G816" t="s">
         <v>27</v>
@@ -36955,7 +36912,7 @@
         <v>4</v>
       </c>
       <c r="F817" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G817" t="s">
         <v>27</v>
@@ -36987,7 +36944,7 @@
         <v>5</v>
       </c>
       <c r="F818" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G818" t="s">
         <v>104</v>
@@ -37019,7 +36976,7 @@
         <v>5</v>
       </c>
       <c r="F819" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G819" t="s">
         <v>104</v>
@@ -37051,7 +37008,7 @@
         <v>5</v>
       </c>
       <c r="F820" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G820" t="s">
         <v>104</v>
@@ -37083,7 +37040,7 @@
         <v>5</v>
       </c>
       <c r="F821" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G821" t="s">
         <v>104</v>
@@ -37115,7 +37072,7 @@
         <v>5</v>
       </c>
       <c r="F822" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G822" t="s">
         <v>104</v>
@@ -37147,7 +37104,7 @@
         <v>5</v>
       </c>
       <c r="F823" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G823" t="s">
         <v>104</v>
@@ -37179,7 +37136,7 @@
         <v>3</v>
       </c>
       <c r="F824" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G824" t="s">
         <v>104</v>
@@ -37211,7 +37168,7 @@
         <v>1</v>
       </c>
       <c r="F825" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G825" t="s">
         <v>104</v>
@@ -37243,7 +37200,7 @@
         <v>1</v>
       </c>
       <c r="F826" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G826" t="s">
         <v>104</v>
@@ -37275,7 +37232,7 @@
         <v>1</v>
       </c>
       <c r="F827" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G827" t="s">
         <v>104</v>
@@ -37307,7 +37264,7 @@
         <v>1</v>
       </c>
       <c r="F828" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G828" t="s">
         <v>104</v>
@@ -37339,7 +37296,7 @@
         <v>1</v>
       </c>
       <c r="F829" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G829" t="s">
         <v>104</v>
@@ -37371,7 +37328,7 @@
         <v>1</v>
       </c>
       <c r="F830" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G830" t="s">
         <v>104</v>
@@ -37403,7 +37360,7 @@
         <v>4</v>
       </c>
       <c r="F831" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G831" t="s">
         <v>104</v>
@@ -37435,7 +37392,7 @@
         <v>3</v>
       </c>
       <c r="F832" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G832" t="s">
         <v>104</v>
@@ -37467,7 +37424,7 @@
         <v>3</v>
       </c>
       <c r="F833" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G833" t="s">
         <v>104</v>
@@ -37499,7 +37456,7 @@
         <v>5</v>
       </c>
       <c r="F834" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G834" t="s">
         <v>104</v>
@@ -37531,7 +37488,7 @@
         <v>3</v>
       </c>
       <c r="F835" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G835" t="s">
         <v>104</v>
@@ -37563,7 +37520,7 @@
         <v>3</v>
       </c>
       <c r="F836" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G836" t="s">
         <v>104</v>
@@ -37595,7 +37552,7 @@
         <v>1</v>
       </c>
       <c r="F837" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G837" t="s">
         <v>104</v>
@@ -37627,7 +37584,7 @@
         <v>2</v>
       </c>
       <c r="F838" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G838" t="s">
         <v>104</v>
@@ -37659,7 +37616,7 @@
         <v>1</v>
       </c>
       <c r="F839" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G839" t="s">
         <v>104</v>
@@ -37691,7 +37648,7 @@
         <v>1</v>
       </c>
       <c r="F840" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G840" t="s">
         <v>104</v>
@@ -37723,7 +37680,7 @@
         <v>4</v>
       </c>
       <c r="F841" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G841" t="s">
         <v>104</v>
@@ -37755,7 +37712,7 @@
         <v>5</v>
       </c>
       <c r="F842" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G842" t="s">
         <v>71</v>
@@ -37787,7 +37744,7 @@
         <v>5</v>
       </c>
       <c r="F843" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G843" t="s">
         <v>71</v>
@@ -37819,7 +37776,7 @@
         <v>5</v>
       </c>
       <c r="F844" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G844" t="s">
         <v>71</v>
@@ -37851,7 +37808,7 @@
         <v>5</v>
       </c>
       <c r="F845" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G845" t="s">
         <v>71</v>
@@ -37883,7 +37840,7 @@
         <v>5</v>
       </c>
       <c r="F846" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G846" t="s">
         <v>71</v>
@@ -37915,7 +37872,7 @@
         <v>5</v>
       </c>
       <c r="F847" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G847" t="s">
         <v>71</v>
@@ -37947,7 +37904,7 @@
         <v>3</v>
       </c>
       <c r="F848" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G848" t="s">
         <v>71</v>
@@ -37979,7 +37936,7 @@
         <v>1</v>
       </c>
       <c r="F849" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G849" t="s">
         <v>71</v>
@@ -38011,7 +37968,7 @@
         <v>1</v>
       </c>
       <c r="F850" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G850" t="s">
         <v>71</v>
@@ -38043,7 +38000,7 @@
         <v>1</v>
       </c>
       <c r="F851" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G851" t="s">
         <v>71</v>
@@ -38075,7 +38032,7 @@
         <v>1</v>
       </c>
       <c r="F852" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G852" t="s">
         <v>71</v>
@@ -38107,7 +38064,7 @@
         <v>1</v>
       </c>
       <c r="F853" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G853" t="s">
         <v>71</v>
@@ -38139,7 +38096,7 @@
         <v>1</v>
       </c>
       <c r="F854" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G854" t="s">
         <v>71</v>
@@ -38171,7 +38128,7 @@
         <v>4</v>
       </c>
       <c r="F855" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G855" t="s">
         <v>71</v>
@@ -38203,7 +38160,7 @@
         <v>3</v>
       </c>
       <c r="F856" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G856" t="s">
         <v>71</v>
@@ -38235,7 +38192,7 @@
         <v>3</v>
       </c>
       <c r="F857" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G857" t="s">
         <v>71</v>
@@ -38267,7 +38224,7 @@
         <v>5</v>
       </c>
       <c r="F858" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G858" t="s">
         <v>71</v>
@@ -38299,7 +38256,7 @@
         <v>3</v>
       </c>
       <c r="F859" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G859" t="s">
         <v>71</v>
@@ -38331,7 +38288,7 @@
         <v>3</v>
       </c>
       <c r="F860" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G860" t="s">
         <v>71</v>
@@ -38363,7 +38320,7 @@
         <v>1</v>
       </c>
       <c r="F861" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G861" t="s">
         <v>71</v>
@@ -38395,7 +38352,7 @@
         <v>2</v>
       </c>
       <c r="F862" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G862" t="s">
         <v>71</v>
@@ -38427,7 +38384,7 @@
         <v>1</v>
       </c>
       <c r="F863" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G863" t="s">
         <v>71</v>
@@ -38459,7 +38416,7 @@
         <v>1</v>
       </c>
       <c r="F864" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G864" t="s">
         <v>71</v>
@@ -38491,7 +38448,7 @@
         <v>4</v>
       </c>
       <c r="F865" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G865" t="s">
         <v>71</v>
@@ -38529,18 +38486,18 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C4" t="s">
         <v>328</v>
@@ -38549,7 +38506,7 @@
         <v>331</v>
       </c>
       <c r="E4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -38928,7 +38885,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B27" s="6">
         <v>-2.1073379999998805</v>
@@ -39023,10 +38980,10 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
+        <v>338</v>
+      </c>
+      <c r="T1" t="s">
         <v>339</v>
-      </c>
-      <c r="T1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
@@ -39100,10 +39057,10 @@
         <v>6.2977000000000005E-2</v>
       </c>
       <c r="AJ2" t="s">
+        <v>338</v>
+      </c>
+      <c r="AK2" t="s">
         <v>339</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -46835,10 +46792,10 @@
         <v>17</v>
       </c>
       <c r="AS1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AT1" t="s">
         <v>339</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>340</v>
       </c>
       <c r="BA1" t="s">
         <v>143</v>
@@ -46859,7 +46816,7 @@
         <v>143</v>
       </c>
       <c r="BI1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.25">
@@ -79447,112 +79404,112 @@
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F26" t="s">
         <v>143</v>
       </c>
       <c r="G26" t="s">
+        <v>340</v>
+      </c>
+      <c r="H26" t="s">
         <v>341</v>
-      </c>
-      <c r="H26" t="s">
-        <v>342</v>
       </c>
       <c r="I26" t="s">
         <v>143</v>
       </c>
       <c r="J26" t="s">
+        <v>340</v>
+      </c>
+      <c r="K26" t="s">
         <v>341</v>
-      </c>
-      <c r="K26" t="s">
-        <v>342</v>
       </c>
       <c r="L26" t="s">
         <v>143</v>
       </c>
       <c r="M26" t="s">
+        <v>340</v>
+      </c>
+      <c r="N26" t="s">
         <v>341</v>
-      </c>
-      <c r="N26" t="s">
-        <v>342</v>
       </c>
       <c r="O26" t="s">
         <v>143</v>
       </c>
       <c r="P26" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q26" t="s">
         <v>341</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>342</v>
       </c>
       <c r="R26" t="s">
         <v>143</v>
       </c>
       <c r="S26" t="s">
+        <v>340</v>
+      </c>
+      <c r="T26" t="s">
         <v>341</v>
-      </c>
-      <c r="T26" t="s">
-        <v>342</v>
       </c>
       <c r="U26" t="s">
         <v>143</v>
       </c>
       <c r="V26" t="s">
+        <v>340</v>
+      </c>
+      <c r="W26" t="s">
         <v>341</v>
-      </c>
-      <c r="W26" t="s">
-        <v>342</v>
       </c>
       <c r="X26" t="s">
         <v>143</v>
       </c>
       <c r="Y26" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z26" t="s">
         <v>341</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>342</v>
       </c>
       <c r="AA26" t="s">
         <v>143</v>
       </c>
       <c r="AB26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AC26" t="s">
         <v>341</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>342</v>
       </c>
       <c r="AD26" t="s">
         <v>143</v>
       </c>
       <c r="AE26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AF26" t="s">
         <v>341</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>342</v>
       </c>
       <c r="AG26" t="s">
         <v>143</v>
       </c>
       <c r="AH26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AI26" t="s">
         <v>341</v>
-      </c>
-      <c r="AI26" t="s">
-        <v>342</v>
       </c>
       <c r="AJ26" t="s">
         <v>143</v>
       </c>
       <c r="AK26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AL26" t="s">
         <v>341</v>
-      </c>
-      <c r="AL26" t="s">
-        <v>342</v>
       </c>
       <c r="AM26" t="s">
         <v>143</v>
       </c>
       <c r="AN26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="5:5" x14ac:dyDescent="0.25">
@@ -82635,112 +82592,112 @@
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G26" t="s">
         <v>143</v>
       </c>
       <c r="H26" t="s">
+        <v>340</v>
+      </c>
+      <c r="I26" t="s">
         <v>341</v>
-      </c>
-      <c r="I26" t="s">
-        <v>342</v>
       </c>
       <c r="J26" t="s">
         <v>143</v>
       </c>
       <c r="K26" t="s">
+        <v>340</v>
+      </c>
+      <c r="L26" t="s">
         <v>341</v>
-      </c>
-      <c r="L26" t="s">
-        <v>342</v>
       </c>
       <c r="M26" t="s">
         <v>143</v>
       </c>
       <c r="N26" t="s">
+        <v>340</v>
+      </c>
+      <c r="O26" t="s">
         <v>341</v>
-      </c>
-      <c r="O26" t="s">
-        <v>342</v>
       </c>
       <c r="P26" t="s">
         <v>143</v>
       </c>
       <c r="Q26" t="s">
+        <v>340</v>
+      </c>
+      <c r="R26" t="s">
         <v>341</v>
-      </c>
-      <c r="R26" t="s">
-        <v>342</v>
       </c>
       <c r="S26" t="s">
         <v>143</v>
       </c>
       <c r="T26" t="s">
+        <v>340</v>
+      </c>
+      <c r="U26" t="s">
         <v>341</v>
-      </c>
-      <c r="U26" t="s">
-        <v>342</v>
       </c>
       <c r="V26" t="s">
         <v>143</v>
       </c>
       <c r="W26" t="s">
+        <v>340</v>
+      </c>
+      <c r="X26" t="s">
         <v>341</v>
-      </c>
-      <c r="X26" t="s">
-        <v>342</v>
       </c>
       <c r="Y26" t="s">
         <v>143</v>
       </c>
       <c r="Z26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AA26" t="s">
         <v>341</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>342</v>
       </c>
       <c r="AB26" t="s">
         <v>143</v>
       </c>
       <c r="AC26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AD26" t="s">
         <v>341</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>342</v>
       </c>
       <c r="AE26" t="s">
         <v>143</v>
       </c>
       <c r="AF26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AG26" t="s">
         <v>341</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>342</v>
       </c>
       <c r="AH26" t="s">
         <v>143</v>
       </c>
       <c r="AI26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AJ26" t="s">
         <v>341</v>
-      </c>
-      <c r="AJ26" t="s">
-        <v>342</v>
       </c>
       <c r="AK26" t="s">
         <v>143</v>
       </c>
       <c r="AL26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AM26" t="s">
         <v>341</v>
-      </c>
-      <c r="AM26" t="s">
-        <v>342</v>
       </c>
       <c r="AN26" t="s">
         <v>143</v>
       </c>
       <c r="AO26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -86722,112 +86679,112 @@
     </row>
     <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="S27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="T27" t="s">
         <v>143</v>
       </c>
       <c r="U27" t="s">
+        <v>340</v>
+      </c>
+      <c r="V27" t="s">
         <v>341</v>
-      </c>
-      <c r="V27" t="s">
-        <v>342</v>
       </c>
       <c r="W27" t="s">
         <v>143</v>
       </c>
       <c r="X27" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y27" t="s">
         <v>341</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>342</v>
       </c>
       <c r="Z27" t="s">
         <v>143</v>
       </c>
       <c r="AA27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB27" t="s">
         <v>341</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>342</v>
       </c>
       <c r="AC27" t="s">
         <v>143</v>
       </c>
       <c r="AD27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE27" t="s">
         <v>341</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>342</v>
       </c>
       <c r="AF27" t="s">
         <v>143</v>
       </c>
       <c r="AG27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AH27" t="s">
         <v>341</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>342</v>
       </c>
       <c r="AI27" t="s">
         <v>143</v>
       </c>
       <c r="AJ27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AK27" t="s">
         <v>341</v>
-      </c>
-      <c r="AK27" t="s">
-        <v>342</v>
       </c>
       <c r="AL27" t="s">
         <v>143</v>
       </c>
       <c r="AM27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AN27" t="s">
         <v>341</v>
-      </c>
-      <c r="AN27" t="s">
-        <v>342</v>
       </c>
       <c r="AO27" t="s">
         <v>143</v>
       </c>
       <c r="AP27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AQ27" t="s">
         <v>341</v>
-      </c>
-      <c r="AQ27" t="s">
-        <v>342</v>
       </c>
       <c r="AR27" t="s">
         <v>143</v>
       </c>
       <c r="AS27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AT27" t="s">
         <v>341</v>
-      </c>
-      <c r="AT27" t="s">
-        <v>342</v>
       </c>
       <c r="AU27" t="s">
         <v>143</v>
       </c>
       <c r="AV27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AW27" t="s">
         <v>341</v>
-      </c>
-      <c r="AW27" t="s">
-        <v>342</v>
       </c>
       <c r="AX27" t="s">
         <v>143</v>
       </c>
       <c r="AY27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AZ27" t="s">
         <v>341</v>
-      </c>
-      <c r="AZ27" t="s">
-        <v>342</v>
       </c>
       <c r="BA27" t="s">
         <v>143</v>
       </c>
       <c r="BB27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:54" x14ac:dyDescent="0.25">
@@ -90787,112 +90744,112 @@
     </row>
     <row r="54" spans="1:54" x14ac:dyDescent="0.25">
       <c r="S54" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="T54" t="s">
         <v>143</v>
       </c>
       <c r="U54" t="s">
+        <v>340</v>
+      </c>
+      <c r="V54" t="s">
         <v>341</v>
-      </c>
-      <c r="V54" t="s">
-        <v>342</v>
       </c>
       <c r="W54" t="s">
         <v>143</v>
       </c>
       <c r="X54" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y54" t="s">
         <v>341</v>
-      </c>
-      <c r="Y54" t="s">
-        <v>342</v>
       </c>
       <c r="Z54" t="s">
         <v>143</v>
       </c>
       <c r="AA54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB54" t="s">
         <v>341</v>
-      </c>
-      <c r="AB54" t="s">
-        <v>342</v>
       </c>
       <c r="AC54" t="s">
         <v>143</v>
       </c>
       <c r="AD54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE54" t="s">
         <v>341</v>
-      </c>
-      <c r="AE54" t="s">
-        <v>342</v>
       </c>
       <c r="AF54" t="s">
         <v>143</v>
       </c>
       <c r="AG54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AH54" t="s">
         <v>341</v>
-      </c>
-      <c r="AH54" t="s">
-        <v>342</v>
       </c>
       <c r="AI54" t="s">
         <v>143</v>
       </c>
       <c r="AJ54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AK54" t="s">
         <v>341</v>
-      </c>
-      <c r="AK54" t="s">
-        <v>342</v>
       </c>
       <c r="AL54" t="s">
         <v>143</v>
       </c>
       <c r="AM54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AN54" t="s">
         <v>341</v>
-      </c>
-      <c r="AN54" t="s">
-        <v>342</v>
       </c>
       <c r="AO54" t="s">
         <v>143</v>
       </c>
       <c r="AP54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AQ54" t="s">
         <v>341</v>
-      </c>
-      <c r="AQ54" t="s">
-        <v>342</v>
       </c>
       <c r="AR54" t="s">
         <v>143</v>
       </c>
       <c r="AS54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AT54" t="s">
         <v>341</v>
-      </c>
-      <c r="AT54" t="s">
-        <v>342</v>
       </c>
       <c r="AU54" t="s">
         <v>143</v>
       </c>
       <c r="AV54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AW54" t="s">
         <v>341</v>
-      </c>
-      <c r="AW54" t="s">
-        <v>342</v>
       </c>
       <c r="AX54" t="s">
         <v>143</v>
       </c>
       <c r="AY54" t="s">
+        <v>340</v>
+      </c>
+      <c r="AZ54" t="s">
         <v>341</v>
-      </c>
-      <c r="AZ54" t="s">
-        <v>342</v>
       </c>
       <c r="BA54" t="s">
         <v>143</v>
       </c>
       <c r="BB54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="55" spans="1:54" x14ac:dyDescent="0.25">
@@ -91336,7 +91293,7 @@
       </c>
       <c r="R58" s="9"/>
       <c r="S58">
-        <f t="shared" ref="S58:AH81" si="4">S31-S4</f>
+        <f t="shared" ref="S58:AH80" si="4">S31-S4</f>
         <v>-14.526683999999999</v>
       </c>
       <c r="T58">
@@ -96172,112 +96129,112 @@
         <v>-3.3444279999998798</v>
       </c>
       <c r="S81" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="T81" t="s">
         <v>143</v>
       </c>
       <c r="U81" t="s">
+        <v>340</v>
+      </c>
+      <c r="V81" t="s">
         <v>341</v>
-      </c>
-      <c r="V81" t="s">
-        <v>342</v>
       </c>
       <c r="W81" t="s">
         <v>143</v>
       </c>
       <c r="X81" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y81" t="s">
         <v>341</v>
-      </c>
-      <c r="Y81" t="s">
-        <v>342</v>
       </c>
       <c r="Z81" t="s">
         <v>143</v>
       </c>
       <c r="AA81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB81" t="s">
         <v>341</v>
-      </c>
-      <c r="AB81" t="s">
-        <v>342</v>
       </c>
       <c r="AC81" t="s">
         <v>143</v>
       </c>
       <c r="AD81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE81" t="s">
         <v>341</v>
-      </c>
-      <c r="AE81" t="s">
-        <v>342</v>
       </c>
       <c r="AF81" t="s">
         <v>143</v>
       </c>
       <c r="AG81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AH81" t="s">
         <v>341</v>
-      </c>
-      <c r="AH81" t="s">
-        <v>342</v>
       </c>
       <c r="AI81" t="s">
         <v>143</v>
       </c>
       <c r="AJ81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AK81" t="s">
         <v>341</v>
-      </c>
-      <c r="AK81" t="s">
-        <v>342</v>
       </c>
       <c r="AL81" t="s">
         <v>143</v>
       </c>
       <c r="AM81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AN81" t="s">
         <v>341</v>
-      </c>
-      <c r="AN81" t="s">
-        <v>342</v>
       </c>
       <c r="AO81" t="s">
         <v>143</v>
       </c>
       <c r="AP81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AQ81" t="s">
         <v>341</v>
-      </c>
-      <c r="AQ81" t="s">
-        <v>342</v>
       </c>
       <c r="AR81" t="s">
         <v>143</v>
       </c>
       <c r="AS81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AT81" t="s">
         <v>341</v>
-      </c>
-      <c r="AT81" t="s">
-        <v>342</v>
       </c>
       <c r="AU81" t="s">
         <v>143</v>
       </c>
       <c r="AV81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AW81" t="s">
         <v>341</v>
-      </c>
-      <c r="AW81" t="s">
-        <v>342</v>
       </c>
       <c r="AX81" t="s">
         <v>143</v>
       </c>
       <c r="AY81" t="s">
+        <v>340</v>
+      </c>
+      <c r="AZ81" t="s">
         <v>341</v>
-      </c>
-      <c r="AZ81" t="s">
-        <v>342</v>
       </c>
       <c r="BA81" t="s">
         <v>143</v>
       </c>
       <c r="BB81" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>